<commit_message>
Update Public Highschool Dataset.xlsx
</commit_message>
<xml_diff>
--- a/Public Highschool Dataset.xlsx
+++ b/Public Highschool Dataset.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Google Drive/DS 2000/Project/Boston-Redlining/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16C11826-CF2A-9E4A-8795-C91AD8A412B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7B6183-908B-814A-AAE4-E9362AD16569}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Public_Schools" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Public_Schools!$A$1:$E$132</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Public_Schools!$A$1:$E$129</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>CITY</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Jamaica Plain</t>
   </si>
   <si>
-    <t>Hyde Park</t>
-  </si>
-  <si>
     <t>Community Academy</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>Lyon, Mary 9-12</t>
   </si>
   <si>
-    <t>Another Course to College</t>
-  </si>
-  <si>
     <t>Brighton High</t>
   </si>
   <si>
@@ -159,9 +153,6 @@
     <t>Horace Mann</t>
   </si>
   <si>
-    <t>New Mission High</t>
-  </si>
-  <si>
     <t>Burke High</t>
   </si>
   <si>
@@ -169,9 +160,6 @@
   </si>
   <si>
     <t>Margarita Muniz Academy</t>
-  </si>
-  <si>
-    <t>Community Leadership Academy</t>
   </si>
   <si>
     <t>Boston Adult Tech Acad</t>
@@ -189,9 +177,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -673,7 +661,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1028,11 +1016,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F132"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1057,72 +1045,72 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>1285</v>
+        <v>1010</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>2136</v>
+        <v>2115</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="E2" s="2">
-        <v>97.6</v>
+        <v>97.4</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>1010</v>
+        <v>1030</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>2115</v>
+        <v>2120</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2">
-        <v>97.4</v>
+        <v>96.6</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>2120</v>
+        <v>2121</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2">
-        <v>96.6</v>
+        <v>95.3</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>1020</v>
+        <v>1440</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5">
-        <v>2121</v>
+        <v>2115</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E5" s="2">
         <v>95.3</v>
@@ -1130,554 +1118,503 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>1440</v>
+        <v>1420</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>2115</v>
+        <v>2122</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2">
-        <v>95.3</v>
+        <v>90.3</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>1420</v>
+        <v>1265</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7">
-        <v>2122</v>
+        <v>2120</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2">
-        <v>90.3</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>1265</v>
+        <v>1460</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>2120</v>
+        <v>2124</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E8" s="2">
-        <v>90</v>
+        <v>88.8</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>1460</v>
+        <v>1450</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>2124</v>
+        <v>2116</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>88.8</v>
+        <v>84.9</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>1450</v>
+        <v>1171</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C10">
-        <v>2116</v>
+        <v>2135</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2">
-        <v>84.9</v>
+        <v>81.3</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>1195</v>
+        <v>1200</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>2136</v>
+        <v>2116</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="E11" s="2">
-        <v>81.7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>1171</v>
+        <v>1260</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C12">
-        <v>2135</v>
+        <v>2119</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E12" s="2">
-        <v>81.3</v>
+        <v>78.900000000000006</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>1200</v>
+        <v>1120</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>2116</v>
+        <v>2121</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E13" s="2">
-        <v>80</v>
+        <v>76.900000000000006</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>1230</v>
+        <v>1070</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>2136</v>
+        <v>2128</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="E14" s="2">
-        <v>79.400000000000006</v>
+        <v>74.7</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>1260</v>
+        <v>1470</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C15">
-        <v>2119</v>
+        <v>2135</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E15" s="2">
-        <v>78.900000000000006</v>
+        <v>74.599999999999994</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>1120</v>
+        <v>1053</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C16">
-        <v>2121</v>
+        <v>2130</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="2">
-        <v>76.900000000000006</v>
+        <v>73.3</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <v>1070</v>
+        <v>1103</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C17">
-        <v>2128</v>
+        <v>2122</v>
       </c>
       <c r="D17" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E17" s="2">
-        <v>74.7</v>
+        <v>72.3</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <v>1470</v>
+        <v>1140</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="C18">
-        <v>2135</v>
+        <v>2124</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="E18" s="2">
-        <v>74.599999999999994</v>
+        <v>70.400000000000006</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <v>1053</v>
+        <v>1162</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C19">
-        <v>2130</v>
+        <v>2127</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="E19" s="2">
-        <v>73.3</v>
+        <v>70.3</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>1103</v>
+        <v>1256</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C20">
-        <v>2122</v>
+        <v>2132</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E20" s="2">
-        <v>72.3</v>
+        <v>63.7</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <v>1140</v>
+        <v>1253</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C21">
-        <v>2124</v>
+        <v>2132</v>
       </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E21" s="2">
-        <v>70.400000000000006</v>
+        <v>61.7</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <v>1162</v>
+        <v>1080</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C22">
-        <v>2127</v>
+        <v>2130</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E22" s="2">
-        <v>70.3</v>
+        <v>60.9</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <v>1256</v>
+        <v>1040</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C23">
-        <v>2132</v>
+        <v>2135</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="E23" s="2">
-        <v>63.7</v>
+        <v>59.3</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <v>1253</v>
+        <v>1210</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C24">
-        <v>2132</v>
+        <v>2120</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="E24" s="2">
-        <v>61.7</v>
+        <v>56.9</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
-        <v>1080</v>
+        <v>1050</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C25">
-        <v>2130</v>
+        <v>2129</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E25" s="2">
-        <v>60.9</v>
+        <v>55.3</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26">
-        <v>1040</v>
+        <v>1430</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C26">
-        <v>2135</v>
+        <v>2119</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E26" s="2">
-        <v>59.3</v>
+        <v>54.5</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
-        <v>1210</v>
+        <v>4610</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C27">
-        <v>2120</v>
+        <v>2134</v>
       </c>
       <c r="D27" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="E27" s="2">
-        <v>56.9</v>
+        <v>44.4</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28">
-        <v>1050</v>
+        <v>1991</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>2129</v>
+        <v>2124</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E28" s="2">
-        <v>55.3</v>
+        <v>43.7</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29">
-        <v>1430</v>
+        <v>1340</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C29">
-        <v>2119</v>
+        <v>2130</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E29" s="2">
-        <v>54.5</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30">
-        <v>4610</v>
+        <v>1293</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="C30">
-        <v>2134</v>
+        <v>2215</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E30" s="2">
-        <v>44.4</v>
+        <v>32.200000000000003</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31">
-        <v>1991</v>
+        <v>1215</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C31">
-        <v>2124</v>
+        <v>2116</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="E31" s="2">
-        <v>43.7</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32">
-        <v>1340</v>
+        <v>1410</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C32">
-        <v>2130</v>
+        <v>2119</v>
       </c>
       <c r="D32" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E32" s="2">
-        <v>35.5</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33">
-        <v>1293</v>
+        <v>4345</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C33">
-        <v>2215</v>
+        <v>2124</v>
       </c>
       <c r="D33" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="E33" s="2">
-        <v>32.200000000000003</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34">
-        <v>1215</v>
-      </c>
-      <c r="B34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34">
-        <v>2116</v>
-      </c>
-      <c r="D34" t="s">
-        <v>47</v>
-      </c>
-      <c r="E34" s="2">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35">
-        <v>1410</v>
-      </c>
-      <c r="B35" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35">
-        <v>2119</v>
-      </c>
-      <c r="D35" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" s="2">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36">
-        <v>4345</v>
-      </c>
-      <c r="B36" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36">
-        <v>2124</v>
-      </c>
-      <c r="D36" t="s">
-        <v>21</v>
-      </c>
-      <c r="E36" s="2">
         <v>9.3000000000000007</v>
       </c>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="F42" s="1"/>
-    </row>
-    <row r="58" spans="6:6">
-      <c r="F58" s="1"/>
-    </row>
-    <row r="82" spans="6:6">
-      <c r="F82" s="1"/>
-    </row>
-    <row r="107" spans="6:6">
-      <c r="F107" s="1"/>
-    </row>
-    <row r="131" spans="6:6">
-      <c r="F131" s="1"/>
-    </row>
-    <row r="132" spans="6:6">
-      <c r="F132" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="F39" s="1"/>
+    </row>
+    <row r="55" spans="6:6">
+      <c r="F55" s="1"/>
+    </row>
+    <row r="79" spans="6:6">
+      <c r="F79" s="1"/>
+    </row>
+    <row r="104" spans="6:6">
+      <c r="F104" s="1"/>
+    </row>
+    <row r="128" spans="6:6">
+      <c r="F128" s="1"/>
+    </row>
+    <row r="129" spans="6:6">
+      <c r="F129" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E132">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E132">
-      <sortCondition descending="1" ref="E1:E132"/>
+  <autoFilter ref="A1:E129" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E129">
+      <sortCondition descending="1" ref="E1:E129"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>